<commit_message>
fixed visuals, updated documentation
</commit_message>
<xml_diff>
--- a/documents/Tabs.xlsx
+++ b/documents/Tabs.xlsx
@@ -20,39 +20,171 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t xml:space="preserve">Tab</t>
   </si>
   <si>
-    <t xml:space="preserve">Subtab</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Subsubtab</t>
+    <t xml:space="preserve">Function</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Description</t>
   </si>
   <si>
     <t xml:space="preserve">AES</t>
   </si>
   <si>
-    <t xml:space="preserve">IV</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pass, ivi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pass, iv</t>
-  </si>
-  <si>
-    <t xml:space="preserve">key, iv</t>
-  </si>
-  <si>
-    <t xml:space="preserve">No IV</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pass</t>
-  </si>
-  <si>
-    <t xml:space="preserve">key</t>
+    <t xml:space="preserve">Password, IV From Hash</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Key: the first 16, 24, or all 32 bytes of the SHA-256 hash of the password
+IV: 16 bytes taken from the SHA-256 hash of the password (0-16)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Password, IV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Key: the first 16, 24, or all 32 bytes of the SHA-256 hash of the password
+IV: 16 bytes provided as a hexadecimal string</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Key, IV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Key: 16, 24, or 32 bytes provided as a hexadecimal string
+IV: 16 bytes provided as a hexadecimal string</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Password, No IV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Key: the first 16, 24, or all 32 bytes of the SHA-256 hash of the password
+IV: none</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Key, No IV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Key: 16, 24, or 32 bytes provided as a hexadecimal string
+IV: none</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SHA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hashing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hashes a text string using SHA-256 and SHA-512</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ECDSA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Generate Keypair</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Erases "Private Key", </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Public Key (X)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">, and </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Public Key (Y)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Generates ECC public and private key and places them in appropriate fields</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Sign</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Erases "Signature (R)", and "Signature (S)"
+Uses ECDSA to sign "Message" with "Private Key", placing R and S in appropriate fields</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verifies signature in R and S with Message and Public Key, displays validation in text box</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Random</t>
+  </si>
+  <si>
+    <t xml:space="preserve">New Number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Generates a random number with the required bytelength
+Displays in Decimal, Hexadecimal, and Base64</t>
   </si>
 </sst>
 </file>
@@ -62,7 +194,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="15"/>
       <name val="Verdana"/>
@@ -90,6 +222,11 @@
       <name val="Verdana"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="15"/>
+      <name val="Verdana"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -134,17 +271,21 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -152,7 +293,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -172,77 +313,131 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
+      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.703125" defaultRowHeight="18.55" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="4.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="7.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="10.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="7.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="20.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="72.43"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="4" style="1" width="6.7"/>
   </cols>
   <sheetData>
-    <row r="1" s="2" customFormat="true" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
+    <row r="1" s="3" customFormat="true" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="s">
+    <row r="2" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3"/>
-      <c r="B3" s="4"/>
-      <c r="C3" s="1" t="s">
+    <row r="3" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="4"/>
+      <c r="B3" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="3"/>
-      <c r="B4" s="4"/>
-      <c r="C4" s="1" t="s">
+      <c r="C3" s="5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="3"/>
-      <c r="B5" s="4" t="s">
+    <row r="4" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="4"/>
+      <c r="B4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C4" s="5" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="3"/>
-      <c r="B6" s="4"/>
-      <c r="C6" s="1" t="s">
+    <row r="5" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="4"/>
+      <c r="B5" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="C5" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="4"/>
+      <c r="B6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B9" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B10" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>26</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="2">
     <mergeCell ref="A2:A6"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="A8:A10"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="0.7875" bottom="0.7875" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>

<commit_message>
reworked ECDSA tab to ECC tab with ECDH and Unpacking functionality, and removed JSeparators
</commit_message>
<xml_diff>
--- a/documents/Tabs.xlsx
+++ b/documents/Tabs.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
   <si>
     <t xml:space="preserve">Tab</t>
   </si>
@@ -78,27 +78,51 @@
     <t xml:space="preserve">Hashes a text string using SHA-256 and SHA-512</t>
   </si>
   <si>
-    <t xml:space="preserve">ECDSA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Generate Keypair</t>
+    <t xml:space="preserve">ECC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Generate Keypair (ECDSA)</t>
   </si>
   <si>
     <t xml:space="preserve">Erases "Private Key", "Public Key (X)", and "Public Key (Y)"
 Generates ECC public and private key and places them in appropriate fields</t>
   </si>
   <si>
-    <t xml:space="preserve">Sign</t>
+    <t xml:space="preserve">Sign (ECDSA)</t>
   </si>
   <si>
     <t xml:space="preserve">Erases "Signature (R)", and "Signature (S)"
 Uses ECDSA to sign "Message" with "Private Key", placing R and S in appropriate fields</t>
   </si>
   <si>
-    <t xml:space="preserve">Verify</t>
+    <t xml:space="preserve">Verify (ECDSA)</t>
   </si>
   <si>
     <t xml:space="preserve">Verifies signature in R and S with Message and Public Key, displays validation in text box</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Multiply (ECDH)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Elliptic curve point multiplication</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Use Generator (ECDH)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sets X and Y to the generator point G</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unpack (Unpacking)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">unpacks the packed public key point</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pack (Unpacking)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">packs the public key point</t>
   </si>
   <si>
     <t xml:space="preserve">Random</t>
@@ -241,16 +265,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C13" activeCellId="0" sqref="C13"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.703125" defaultRowHeight="18.55" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="7.54"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="20.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="22.65"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="72.43"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="4" style="1" width="6.7"/>
   </cols>
@@ -353,32 +377,71 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1" t="s">
+    <row r="11" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="4"/>
+      <c r="B11" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="C11" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C11" s="5" t="s">
+    </row>
+    <row r="12" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="4"/>
+      <c r="B12" s="1" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="12" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="1" t="s">
+      <c r="C12" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B12" s="1" t="s">
+    </row>
+    <row r="13" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="4"/>
+      <c r="B13" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C13" s="5" t="s">
         <v>29</v>
       </c>
+    </row>
+    <row r="14" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="4"/>
+      <c r="B14" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C17" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A2:A6"/>
-    <mergeCell ref="A8:A10"/>
+    <mergeCell ref="A8:A14"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="0.7875" bottom="0.7875" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>